<commit_message>
Correcao do teste solicitado pela Spread
</commit_message>
<xml_diff>
--- a/TesteUIPathSpread/Entrada_Dados.xlsx
+++ b/TesteUIPathSpread/Entrada_Dados.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danil\Documents\UiPath\TesteUIPathSpread\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CFB9C1B-AF67-496E-B5AA-C0393BA81F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68237574-6518-410E-AAF7-F5EC5CAAF630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1824" yWindow="2664" windowWidth="17244" windowHeight="8868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Dados!$A:$E</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Dados!$A$1:$E$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>CPF</t>
   </si>
@@ -68,12 +68,6 @@
   </si>
   <si>
     <t>15/11/1979</t>
-  </si>
-  <si>
-    <t>420,00</t>
-  </si>
-  <si>
-    <t>610,00</t>
   </si>
 </sst>
 </file>
@@ -114,19 +108,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -427,7 +409,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD1048575"/>
+      <selection activeCell="A4" sqref="A4:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -466,8 +448,8 @@
       <c r="D2">
         <v>650</v>
       </c>
-      <c r="E2" t="s">
-        <v>11</v>
+      <c r="E2">
+        <v>420</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -483,15 +465,12 @@
       <c r="D3">
         <v>100</v>
       </c>
-      <c r="E3" t="s">
-        <v>12</v>
+      <c r="E3">
+        <v>610</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1048575" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
+  <autoFilter ref="A1:E3" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
 </file>
</xml_diff>